<commit_message>
Added dolphin build to repo to run from command line
</commit_message>
<xml_diff>
--- a/Evaluation/Lap_Times.xlsx
+++ b/Evaluation/Lap_Times.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\Documents\3rd Year\Project\my-project\Evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Users\Harry Stevenson\Documents\project\hjs115\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775F08B9-E490-4AB1-B888-A00266DF9FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAE36C9-5D74-4971-ADE7-A7A3BC0C4892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6125C1F9-BBBE-4F59-A392-2113E9B410CB}"/>
+    <workbookView minimized="1" xWindow="5310" yWindow="435" windowWidth="9675" windowHeight="14550" xr2:uid="{6125C1F9-BBBE-4F59-A392-2113E9B410CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Tom</t>
+  </si>
+  <si>
+    <t>Thomas S</t>
   </si>
 </sst>
 </file>
@@ -139,6 +142,31 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7EC9BB5F-4998-4CBD-871B-9A1866A95995}" name="Table1" displayName="Table1" ref="A1:G12" totalsRowShown="0">
+  <autoFilter ref="A1:G12" xr:uid="{7EC9BB5F-4998-4CBD-871B-9A1866A95995}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
+    <sortCondition ref="G1:G12"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{01BB8787-FA06-45F1-8251-54DD0EFADE08}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{15BAD7F8-41C7-4279-84E6-D67B4FB8117A}" name="Lap 1"/>
+    <tableColumn id="3" xr3:uid="{8A1F96A4-247D-442F-8889-04C4FB399148}" name="Lap 2"/>
+    <tableColumn id="4" xr3:uid="{D503BD53-413A-4476-B829-607325C05130}" name="Lap 3 "/>
+    <tableColumn id="5" xr3:uid="{E9337D50-607D-4954-90FA-DA429B3BCB28}" name="Best">
+      <calculatedColumnFormula>MIN(B2:D2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{190BC469-480C-4941-ADEF-CC83E02EA3F1}" name="Average">
+      <calculatedColumnFormula>AVERAGE(B2:D2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{0A54868E-05A5-4136-9900-FD6A3DAA13E7}" name="TOTAL">
+      <calculatedColumnFormula>SUM(B2:D2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -438,15 +466,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F4D2C6-7871-45C3-A606-4DC51E29BE78}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,137 +500,137 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B2">
-        <v>33.497999999999998</v>
+        <v>34.615000000000002</v>
       </c>
       <c r="C2">
-        <v>34.121000000000002</v>
+        <v>31.155000000000001</v>
       </c>
       <c r="D2">
-        <v>31.635999999999999</v>
+        <v>31.024999999999999</v>
       </c>
       <c r="E2">
         <f>MIN(B2:D2)</f>
-        <v>31.635999999999999</v>
+        <v>31.024999999999999</v>
       </c>
       <c r="F2">
         <f>AVERAGE(B2:D2)</f>
-        <v>33.085000000000001</v>
+        <v>32.265000000000008</v>
       </c>
       <c r="G2">
         <f>SUM(B2:D2)</f>
-        <v>99.254999999999995</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>96.795000000000016</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>38.292999999999999</v>
+        <v>33.497999999999998</v>
       </c>
       <c r="C3">
-        <v>32.747</v>
+        <v>34.121000000000002</v>
       </c>
       <c r="D3">
-        <v>32.518999999999998</v>
+        <v>31.635999999999999</v>
       </c>
       <c r="E3">
         <f>MIN(B3:D3)</f>
-        <v>32.518999999999998</v>
+        <v>31.635999999999999</v>
       </c>
       <c r="F3">
         <f>AVERAGE(B3:D3)</f>
+        <v>33.085000000000001</v>
+      </c>
+      <c r="G3">
+        <f>SUM(B3:D3)</f>
+        <v>99.254999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>35.39</v>
+      </c>
+      <c r="C4">
+        <v>33.652999999999999</v>
+      </c>
+      <c r="D4">
+        <v>31.655000000000001</v>
+      </c>
+      <c r="E4">
+        <f>MIN(B4:D4)</f>
+        <v>31.655000000000001</v>
+      </c>
+      <c r="F4">
+        <f>AVERAGE(B4:D4)</f>
+        <v>33.566000000000003</v>
+      </c>
+      <c r="G4">
+        <f>SUM(B4:D4)</f>
+        <v>100.69800000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>35.798000000000002</v>
+      </c>
+      <c r="C5">
+        <v>34.921999999999997</v>
+      </c>
+      <c r="D5">
+        <v>31.908000000000001</v>
+      </c>
+      <c r="E5">
+        <f>MIN(B5:D5)</f>
+        <v>31.908000000000001</v>
+      </c>
+      <c r="F5">
+        <f>AVERAGE(B5:D5)</f>
+        <v>34.209333333333333</v>
+      </c>
+      <c r="G5">
+        <f>SUM(B5:D5)</f>
+        <v>102.628</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>38.292999999999999</v>
+      </c>
+      <c r="C6">
+        <v>32.747</v>
+      </c>
+      <c r="D6">
+        <v>32.518999999999998</v>
+      </c>
+      <c r="E6">
+        <f>MIN(B6:D6)</f>
+        <v>32.518999999999998</v>
+      </c>
+      <c r="F6">
+        <f>AVERAGE(B6:D6)</f>
         <v>34.519666666666666</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G11" si="0">SUM(B3:D3)</f>
+      <c r="G6">
+        <f>SUM(B6:D6)</f>
         <v>103.559</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>39.118000000000002</v>
-      </c>
-      <c r="C4">
-        <v>39.020000000000003</v>
-      </c>
-      <c r="D4">
-        <v>33.878999999999998</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E11" si="1">MIN(B4:D4)</f>
-        <v>33.878999999999998</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F11" si="2">AVERAGE(B4:D4)</f>
-        <v>37.338999999999999</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>112.017</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>39.865000000000002</v>
-      </c>
-      <c r="C5">
-        <v>36.329000000000001</v>
-      </c>
-      <c r="D5">
-        <v>36.896999999999998</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>36.329000000000001</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="2"/>
-        <v>37.697000000000003</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>113.09100000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>37.399000000000001</v>
-      </c>
-      <c r="C6">
-        <v>36.807000000000002</v>
-      </c>
-      <c r="D6">
-        <v>40.155999999999999</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>36.807000000000002</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="2"/>
-        <v>38.120666666666665</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>114.36199999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -613,123 +644,152 @@
         <v>34.5</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
+        <f>MIN(B7:D7)</f>
         <v>34.5</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(B7:D7)</f>
         <v>35.854666666666667</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>SUM(B7:D7)</f>
         <v>107.56399999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>39.118000000000002</v>
+      </c>
+      <c r="C8">
+        <v>39.020000000000003</v>
+      </c>
+      <c r="D8">
+        <v>33.878999999999998</v>
+      </c>
+      <c r="E8">
+        <f>MIN(B8:D8)</f>
+        <v>33.878999999999998</v>
+      </c>
+      <c r="F8">
+        <f>AVERAGE(B8:D8)</f>
+        <v>37.338999999999999</v>
+      </c>
+      <c r="G8">
+        <f>SUM(B8:D8)</f>
+        <v>112.017</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>39.865000000000002</v>
+      </c>
+      <c r="C9">
+        <v>36.329000000000001</v>
+      </c>
+      <c r="D9">
+        <v>36.896999999999998</v>
+      </c>
+      <c r="E9">
+        <f>MIN(B9:D9)</f>
+        <v>36.329000000000001</v>
+      </c>
+      <c r="F9">
+        <f>AVERAGE(B9:D9)</f>
+        <v>37.697000000000003</v>
+      </c>
+      <c r="G9">
+        <f>SUM(B9:D9)</f>
+        <v>113.09100000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>37.399000000000001</v>
+      </c>
+      <c r="C10">
+        <v>36.807000000000002</v>
+      </c>
+      <c r="D10">
+        <v>40.155999999999999</v>
+      </c>
+      <c r="E10">
+        <f>MIN(B10:D10)</f>
+        <v>36.807000000000002</v>
+      </c>
+      <c r="F10">
+        <f>AVERAGE(B10:D10)</f>
+        <v>38.120666666666665</v>
+      </c>
+      <c r="G10">
+        <f>SUM(B10:D10)</f>
+        <v>114.36199999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
+      <c r="B11">
         <v>39.762</v>
       </c>
-      <c r="C8">
+      <c r="C11">
         <v>37.948</v>
       </c>
-      <c r="D8">
+      <c r="D11">
         <v>38.109000000000002</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
+      <c r="E11">
+        <f>MIN(B11:D11)</f>
         <v>37.948</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="2"/>
+      <c r="F11">
+        <f>AVERAGE(B11:D11)</f>
         <v>38.606333333333339</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
+      <c r="G11">
+        <f>SUM(B11:D11)</f>
         <v>115.81900000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>35.39</v>
-      </c>
-      <c r="C9">
-        <v>33.652999999999999</v>
-      </c>
-      <c r="D9">
-        <v>31.655000000000001</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>31.655000000000001</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
-        <v>33.566000000000003</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>100.69800000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>35.798000000000002</v>
-      </c>
-      <c r="C10">
-        <v>34.921999999999997</v>
-      </c>
-      <c r="D10">
-        <v>31.908000000000001</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>31.908000000000001</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="2"/>
-        <v>34.209333333333333</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>102.628</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>51.091000000000001</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>36.478999999999999</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>34.97</v>
       </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
+      <c r="E12">
+        <f>MIN(B12:D12)</f>
         <v>34.97</v>
       </c>
-      <c r="F11">
-        <f t="shared" si="2"/>
+      <c r="F12">
+        <f>AVERAGE(B12:D12)</f>
         <v>40.846666666666664</v>
       </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
+      <c r="G12">
+        <f>SUM(B12:D12)</f>
         <v>122.53999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>